<commit_message>
Updated Projects and Emi calc
</commit_message>
<xml_diff>
--- a/private/contacts.xlsx
+++ b/private/contacts.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,54 @@
   </si>
   <si>
     <t>4/3/2025, 5:27:09 pm</t>
+  </si>
+  <si>
+    <t>rihan</t>
+  </si>
+  <si>
+    <t>9684751485</t>
+  </si>
+  <si>
+    <t>Hello i need home</t>
+  </si>
+  <si>
+    <t>8/3/2025, 1:07:42 pm</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>2545487474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homeless guy want some home </t>
+  </si>
+  <si>
+    <t>11/3/2025, 2:20:47 pm</t>
+  </si>
+  <si>
+    <t>mohan pai</t>
+  </si>
+  <si>
+    <t>9845444444</t>
+  </si>
+  <si>
+    <t>Joe less home</t>
+  </si>
+  <si>
+    <t>27/3/2025, 12:12:52 pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richard </t>
+  </si>
+  <si>
+    <t>9854747474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apartment purchase in bc road required we want home to live </t>
+  </si>
+  <si>
+    <t>27/3/2025, 1:09:26 pm</t>
   </si>
 </sst>
 </file>
@@ -444,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -515,6 +563,74 @@
         <v>18</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>